<commit_message>
updated the sheet name
</commit_message>
<xml_diff>
--- a/Branch_Daily_Sales_Report_Sample.xlsx
+++ b/Branch_Daily_Sales_Report_Sample.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="JUL" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="REPORT" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -820,10 +820,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="N1" activeCellId="0" sqref="N1"/>
       <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AK3" activeCellId="0" sqref="AK3:AL6"/>
+      <selection pane="bottomRight" activeCell="AK3" activeCellId="0" sqref="AK3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.5"/>
@@ -833,7 +833,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="8.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="10.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="10.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="0" width="6.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="5.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="6.87"/>

</xml_diff>